<commit_message>
end of day-3 code
</commit_message>
<xml_diff>
--- a/Application API URLs.xlsx
+++ b/Application API URLs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\microservices_training_sasken\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sasken-microservices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -99,6 +99,57 @@
   </si>
   <si>
     <t>deletes an existing basket with given user name</t>
+  </si>
+  <si>
+    <t>ORDERING API</t>
+  </si>
+  <si>
+    <t>api/v1/Order</t>
+  </si>
+  <si>
+    <t>Get orders for given username</t>
+  </si>
+  <si>
+    <t>post order (just for testing-will not be used actually)</t>
+  </si>
+  <si>
+    <t>API GATEWAY MICROSERVICE</t>
+  </si>
+  <si>
+    <t>/Catalog</t>
+  </si>
+  <si>
+    <t>api/v1/Catalog (Post)</t>
+  </si>
+  <si>
+    <t>api/v1/Catalog (Get)</t>
+  </si>
+  <si>
+    <t>/Catalog/{id}</t>
+  </si>
+  <si>
+    <t>/Basket</t>
+  </si>
+  <si>
+    <t>api/v1/Basket (Get)</t>
+  </si>
+  <si>
+    <t>api/v1/Basket (Post)</t>
+  </si>
+  <si>
+    <t>/Basket/Ckeckout</t>
+  </si>
+  <si>
+    <t>api/v1/Basket/Ckeckout (Post)</t>
+  </si>
+  <si>
+    <t>/Order</t>
+  </si>
+  <si>
+    <t>api/v1/Catalog/GetProductByName/{productName}</t>
+  </si>
+  <si>
+    <t>Get matching products given the productName</t>
   </si>
 </sst>
 </file>
@@ -120,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +187,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,13 +245,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -466,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,155 +552,303 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
end of session day -4
</commit_message>
<xml_diff>
--- a/Application API URLs.xlsx
+++ b/Application API URLs.xlsx
@@ -541,7 +541,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>22</v>

</xml_diff>